<commit_message>
Read symbols from text file, add winline and reel bounce
</commit_message>
<xml_diff>
--- a/TheoreticalRTP.xlsx
+++ b/TheoreticalRTP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.stringer\source\repos\JohnsSuperSlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C92DF25F-A574-4648-9E63-E28BAC2783A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D46954-2DC4-4D81-ACBE-0CFB827C3E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{156F91E9-84DF-4BA4-9F8D-39EBB2FA11A0}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -441,7 +440,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>